<commit_message>
avgCsd14 and totalCsd14 over season
</commit_message>
<xml_diff>
--- a/results/Player_Stats_2024-04-27.xlsx
+++ b/results/Player_Stats_2024-04-27.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,15 +491,20 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>csd14</t>
+          <t>totalCsd14</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>avgCsd14</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>first_blood</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>solo_kills</t>
         </is>
@@ -550,9 +555,12 @@
         <v>14</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -601,9 +609,12 @@
         <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -652,9 +663,12 @@
         <v>57</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>28.5</v>
       </c>
       <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -703,9 +717,12 @@
         <v>-59</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>-29.5</v>
       </c>
       <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -754,9 +771,12 @@
         <v>-8</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -805,9 +825,12 @@
         <v>-14</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -856,9 +879,12 @@
         <v>-1</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -907,9 +933,12 @@
         <v>-57</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>-28.5</v>
       </c>
       <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
         <v>3</v>
       </c>
     </row>
@@ -958,9 +987,12 @@
         <v>59</v>
       </c>
       <c r="N10" t="n">
-        <v>2</v>
+        <v>29.5</v>
       </c>
       <c r="O10" t="n">
+        <v>2</v>
+      </c>
+      <c r="P10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1009,9 +1041,12 @@
         <v>8</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1060,9 +1095,12 @@
         <v>-61</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>-30.5</v>
       </c>
       <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1111,11 +1149,14 @@
         <v>35</v>
       </c>
       <c r="N13" t="n">
-        <v>1</v>
+        <v>17.5</v>
       </c>
       <c r="O13" t="n">
         <v>1</v>
       </c>
+      <c r="P13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1162,9 +1203,12 @@
         <v>-47</v>
       </c>
       <c r="N14" t="n">
+        <v>-23.5</v>
+      </c>
+      <c r="O14" t="n">
         <v>1</v>
       </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1213,9 +1257,12 @@
         <v>6</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1264,9 +1311,12 @@
         <v>-19</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>-9.5</v>
       </c>
       <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1315,9 +1365,12 @@
         <v>61</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>30.5</v>
       </c>
       <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1366,9 +1419,12 @@
         <v>-35</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>-17.5</v>
       </c>
       <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1417,9 +1473,12 @@
         <v>47</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>23.5</v>
       </c>
       <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1468,9 +1527,12 @@
         <v>-6</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1519,9 +1581,12 @@
         <v>19</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>